<commit_message>
toelichting and improved geometry
</commit_message>
<xml_diff>
--- a/src/migrations/micro-migratie-rxmission/test/geometries_to_test.xlsx
+++ b/src/migrations/micro-migratie-rxmission/test/geometries_to_test.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wietekekremer/dev/webformulieren-submissionstorage/src/migrations/micro-migratie-rxmission/test/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75849D8-6D1F-C741-BD6D-502876F0C754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="760" windowWidth="27980" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Gegevens"/>
+    <sheet name="Gegevens" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="BronData">Gegevens!$A$1:$B$13</definedName>
   </definedNames>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>openwavezaaknummer</t>
   </si>
@@ -84,12 +90,19 @@
     "coordinates": [ [188819.23, 430662.31], [188871.04, 430736.05], [188869.04, 430729.71], [188860.71, 430713.4], [188857.63, 430708.69], [188854.37, 430703.08], [188851.29, 430697.64], [188841.15, 430683.33], [188836.98, 430678.62], [188824.3, 430665.94], [188814.88, 430659.42], [188809.44, 430655.61] ]
     },</t>
   </si>
+  <si>
+    <t xml:space="preserve">  { "type": "MultiPolygon",
+    "coordinates": [
+      [ [ [187789,429134], [187788,429127], [187794,429128], [187794,429134], [187789,429134] ] ],
+      [ [ [187790,429134], [187789,429117], [187789,429117], [187792,429117], [187793,429117], [187794,429133], [187793,429133], [187793,429134], [187790,429134] ] ]
+      ]
+    },</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -119,26 +132,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -149,10 +160,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -190,71 +201,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -282,7 +293,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -305,11 +316,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -318,13 +329,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -334,7 +345,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -343,7 +354,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -352,7 +363,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -360,10 +371,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -428,122 +439,132 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B24" sqref="B16:B24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="3" width="22.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="60.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="62.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:2" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="62.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:2" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="62.25">
-      <c r="A5" s="2">
+    <row r="5" spans="1:2" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="62.25">
-      <c r="A6" s="2">
+    <row r="6" spans="1:2" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="39.75">
-      <c r="A7" s="2">
+    <row r="7" spans="1:2" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="2">
+    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
-      <c r="A9" s="2">
+    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="39.75">
-      <c r="A10" s="2">
+    <row r="10" spans="1:2" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
-      <c r="A11" s="2">
+    <row r="11" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="39.75">
-      <c r="A12" s="2">
+    <row r="12" spans="1:2" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="39.75">
-      <c r="A13" s="2">
+    <row r="13" spans="1:2" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="144" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dealt with geometry errors in api call
</commit_message>
<xml_diff>
--- a/src/migrations/micro-migratie-rxmission/test/geometries_to_test.xlsx
+++ b/src/migrations/micro-migratie-rxmission/test/geometries_to_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wietekekremer/dev/webformulieren-submissionstorage/src/migrations/micro-migratie-rxmission/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75849D8-6D1F-C741-BD6D-502876F0C754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4F4A82-8747-5B41-A0C4-1C40C6EF1655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="760" windowWidth="27980" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>openwavezaaknummer</t>
   </si>
@@ -97,6 +97,27 @@
       [ [ [187790,429134], [187789,429117], [187789,429117], [187792,429117], [187793,429117], [187794,429133], [187793,429133], [187793,429134], [187790,429134] ] ]
       ]
     },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  { "type": "Polygon",
+    "coordinates": [
+      [ [187671,429084], [187663,429060], [187660,429050], [187683,429031], [187695,429024], [187695,429024], [187695,429025], [187697,429031], [187697,429031], [187697,429031], [187697,429032], [187698,429035], [187699,429035], [187699,429035], [187698,429035], [187699,429036], [187698,429036], [187700,429040], [187697,429041], [187697,429042], [187693,429043], [187693,429045], [187689,429046], [187690,429048], [187686,429049], [187686,429050], [187682,429051], [187679,429052], [187680,429053], [187679,429054], [187687,429079], [187682,429081], [187671,429084] ]
+      ]
+   },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  { "type": "Polygon",
+    "coordinates": [
+      [ [186752,427771], [186708,427744], [186712,427737], [186718,427726], [186797,427774], [186806,427791], [186814,427806], [186817,427811], [186820,427818], [186821,427821], [186816,427824], [186819,427831], [186831,427854], [186834,427859], [186806,427811], [186797,427816], [186799,427818], [186794,427820], [186800,427831], [186781,427837], [186798,427885], [186809,427910], [186821,427934], [186837,427981], [186854,428031], [186899,428172], [186906,428191], [186907,428196], [186904,428197], [186907,428212], [186920,428270], [186922,428281], [186919,428276], [186909,428259], [186905,428240], [186900,428220], [186894,428191], [186884,428161], [186880,428151], [186870,428117], [186859,428085], [186850,428055], [186847,428047], [186846,428043], [186841,428029], [186831,428000], [186821,427972], [186813,427948], [186807,427939], [186796,427920], [186790,427910], [186784,427896], [186778,427880], [186777,427879], [186782,427877], [186789,427874], [186788,427873], [186778,427846], [186772,427834], [186773,427833], [186789,427819], [186795,427808], [186800,427801], [186780,427788], [186780,427788], [186765,427779], [186765,427780], [186752,427771] ]
+      ]
+   },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  { "type": "Polygon",
+    "coordinates": [
+      [ [187017,425818], [186960,425835], [186945,425839], [186931,425784], [186931,425784], [186931,425783], [186931,425783], [186931,425782], [186932,425782], [186932,425781], [186932,425781], [186933,425780], [186933,425780], [186933,425780], [186934,425779], [186934,425779], [186953,425775], [186969,425771], [186984,425768], [187000,425766], [187017,425765], [187016,425765], [187015,425765], [187015,425765], [187014,425766], [187014,425767], [187013,425768], [187014,425769], [187018,425793], [187021,425810], [187018,425811], [187015,425811], [187016,425813], [187017,425818] ]
+      ]
+   },</t>
   </si>
 </sst>
 </file>
@@ -443,10 +464,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B24" sqref="B16:B24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -567,6 +588,46 @@
         <v>14</v>
       </c>
     </row>
+    <row r="15" spans="1:2" ht="144" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>